<commit_message>
Apply button now erases previous inputs to reduce chances of ov erwriting existing stamps
</commit_message>
<xml_diff>
--- a/Work/Templates/transmittal1.xlsx
+++ b/Work/Templates/transmittal1.xlsx
@@ -309,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -359,7 +359,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -399,49 +398,49 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -715,7 +714,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -726,7 +725,7 @@
   <dimension ref="A5:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,16 +754,16 @@
       <c r="H5" s="19"/>
     </row>
     <row r="8" spans="1:12" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
     </row>
     <row r="9" spans="1:12" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
@@ -788,87 +787,87 @@
       <c r="H10" s="11"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="36" t="s">
+      <c r="C11" s="34"/>
+      <c r="D11" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="37">
         <f ca="1">TODAY()</f>
-        <v>42485</v>
-      </c>
-      <c r="F11" s="34" t="s">
+        <v>42486</v>
+      </c>
+      <c r="F11" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="43" t="s">
+      <c r="G11" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="43"/>
+      <c r="H11" s="46"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35" t="s">
+      <c r="A12" s="34"/>
+      <c r="B12" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="34" t="s">
+      <c r="C12" s="34"/>
+      <c r="D12" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="47" t="s">
+      <c r="E12" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
       <c r="J12" s="6"/>
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35" t="s">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="34" t="s">
+      <c r="C13" s="34"/>
+      <c r="D13" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
       <c r="J13" s="6"/>
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35" t="s">
+      <c r="A14" s="34"/>
+      <c r="B14" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="35"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="11"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
       <c r="J14" s="6"/>
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
       <c r="J15" s="6"/>
       <c r="L15" s="6"/>
     </row>
@@ -885,9 +884,6 @@
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="9"/>
@@ -897,7 +893,9 @@
       <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+      <c r="A18" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="B18" s="10"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -906,30 +904,20 @@
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="22" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
+      <c r="B20" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="50" t="s">
+      <c r="C20" s="23"/>
+      <c r="D20" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="51"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="22" t="s">
+      <c r="E20" s="54"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="22"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="22"/>
       <c r="H20" s="22"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -937,7 +925,7 @@
       <c r="B21" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="26"/>
+      <c r="C21" s="25"/>
       <c r="D21" s="22" t="s">
         <v>18</v>
       </c>
@@ -965,13 +953,13 @@
       <c r="H22" s="22"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="27" t="s">
+      <c r="A23" s="25"/>
+      <c r="B23" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
       <c r="F23" s="24"/>
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
@@ -1023,96 +1011,96 @@
       <c r="B28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="49" t="s">
+      <c r="C28" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
       <c r="H28" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="55"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="40"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="39"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="56"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="39"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="38"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="56"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="39"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="38"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="56"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="39"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="38"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="56"/>
-      <c r="B33" s="39"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="39"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="38"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="56"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="39"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="38"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="56"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="39"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="38"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="56"/>
-      <c r="B36" s="39"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="39"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="38"/>
     </row>
     <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
@@ -1137,120 +1125,120 @@
       <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
-      <c r="B39" s="27" t="s">
+      <c r="A39" s="28"/>
+      <c r="B39" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="44" t="s">
+      <c r="C39" s="29"/>
+      <c r="D39" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="E39" s="44"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="45" t="s">
+      <c r="E39" s="49"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="H39" s="46"/>
+      <c r="H39" s="51"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
-      <c r="B40" s="27" t="s">
+      <c r="A40" s="28"/>
+      <c r="B40" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="44" t="s">
+      <c r="C40" s="29"/>
+      <c r="D40" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="E40" s="44"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="45" t="s">
+      <c r="E40" s="49"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="H40" s="46"/>
+      <c r="H40" s="51"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
-      <c r="B41" s="27" t="s">
+      <c r="A41" s="28"/>
+      <c r="B41" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="30"/>
-      <c r="D41" s="44" t="s">
+      <c r="C41" s="29"/>
+      <c r="D41" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="E41" s="44"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="45" t="s">
+      <c r="E41" s="49"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="H41" s="46"/>
+      <c r="H41" s="51"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
-      <c r="B42" s="27" t="s">
+      <c r="A42" s="28"/>
+      <c r="B42" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C42" s="27"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
       <c r="F42" s="22"/>
       <c r="G42" s="22"/>
       <c r="H42" s="22"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
-      <c r="B43" s="27" t="s">
+      <c r="A43" s="28"/>
+      <c r="B43" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="30"/>
-      <c r="D43" s="50" t="s">
+      <c r="C43" s="29"/>
+      <c r="D43" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="54"/>
-      <c r="F43" s="54"/>
-      <c r="G43" s="54"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
       <c r="H43" s="22"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
+      <c r="A44" s="31"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
       <c r="F44" s="22"/>
       <c r="G44" s="22"/>
       <c r="H44" s="22"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="42" t="s">
+      <c r="A45" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="42"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="55"/>
+      <c r="H45" s="55"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="42"/>
-      <c r="B46" s="42"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
+      <c r="A46" s="55"/>
+      <c r="B46" s="55"/>
+      <c r="C46" s="55"/>
+      <c r="D46" s="55"/>
+      <c r="E46" s="55"/>
+      <c r="F46" s="55"/>
+      <c r="G46" s="55"/>
+      <c r="H46" s="55"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="42"/>
-      <c r="B47" s="42"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="42"/>
-      <c r="F47" s="42"/>
-      <c r="G47" s="42"/>
-      <c r="H47" s="42"/>
+      <c r="A47" s="55"/>
+      <c r="B47" s="55"/>
+      <c r="C47" s="55"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="55"/>
+      <c r="F47" s="55"/>
+      <c r="G47" s="55"/>
+      <c r="H47" s="55"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
@@ -1262,9 +1250,9 @@
       <c r="E48" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="33"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="21"/>
@@ -1288,6 +1276,19 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="A45:H47"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
@@ -1296,26 +1297,13 @@
     <mergeCell ref="E12:H12"/>
     <mergeCell ref="E13:H13"/>
     <mergeCell ref="G11:H11"/>
-    <mergeCell ref="D43:G43"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
     <mergeCell ref="E14:H14"/>
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="C28:G28"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="A45:H47"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="D20:E20"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.25" bottom="0.25" header="0" footer="0.25"/>
-  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>